<commit_message>
1) update CRS version (V1.2)
2) edit RTM
3) add link of SIQ doc
</commit_message>
<xml_diff>
--- a/SWE/Software Specification/RTM/RTM.xlsx
+++ b/SWE/Software Specification/RTM/RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti 9 months\Software eng\git\Sovy---Digital-Calculator-PO1_DGC\SWE\Software Specification\RTM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Sovy\Sovy---Digital-Calculator-PO1_DGC\SWE\Software Specification\RTM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>CRS_Requirement_ID</t>
   </si>
@@ -38,15 +38,9 @@
     <t>Req_1ST123_CRS_overall_001-V1.0</t>
   </si>
   <si>
-    <t>Req_1ST123_CRS_overall_002-V1.0</t>
-  </si>
-  <si>
     <t>Req_1ST123_CRS_overall_003-V1.0</t>
   </si>
   <si>
-    <t>Req_1ST123_CRS_overall_004-V1.0</t>
-  </si>
-  <si>
     <t>CR_Requirment_ID</t>
   </si>
   <si>
@@ -59,11 +53,23 @@
     <t>Req_1ST123_CR_overall_02-V1.0</t>
   </si>
   <si>
-    <t>Req_1ST123_CR_overall_04-V1.0</t>
-  </si>
-  <si>
-    <t>Req_1ST123_HSI_overall_001-V1.0
-Req_1ST123_HSI_overall_002-V1.0</t>
+    <t>Req_1ST123_CRS_overall_002-V1.1</t>
+  </si>
+  <si>
+    <t>Req_1ST123_CRS_overall_004-V1.1</t>
+  </si>
+  <si>
+    <t>Req_1ST123_CR_overall_04-V1.1</t>
+  </si>
+  <si>
+    <t>Req_1ST123_HSI_overall_003-V1.0
+Req_1ST123_HSI_overall_004-V1.0</t>
+  </si>
+  <si>
+    <t>Req_1ST123_HSI_overall_005-V1.0</t>
+  </si>
+  <si>
+    <t>Req_1ST123_HSI_overall_002-V1.0</t>
   </si>
 </sst>
 </file>
@@ -200,6 +206,8 @@
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -240,8 +248,6 @@
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -259,12 +265,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C5" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:C5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
   <autoFilter ref="A1:C5"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="CR_Requirment_ID" dataDxfId="4"/>
-    <tableColumn id="2" name="CRS_Requirement_ID" dataDxfId="3"/>
-    <tableColumn id="3" name="HSI_Requirment_ID" dataDxfId="2"/>
+    <tableColumn id="1" name="CR_Requirment_ID" dataDxfId="2"/>
+    <tableColumn id="2" name="CRS_Requirement_ID" dataDxfId="1"/>
+    <tableColumn id="3" name="HSI_Requirment_ID" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -536,21 +542,21 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="40.5546875" style="6" customWidth="1"/>
     <col min="2" max="2" width="46" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="43.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -560,51 +566,51 @@
       </c>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D5" s="4"/>
     </row>

</xml_diff>